<commit_message>
commit layout Guard Tour System step2 (#496)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/上海地区住宅-安防配置表.xlsx
+++ b/AutoLoader/Contents/Support/上海地区住宅-安防配置表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="视频监控系统配置表" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="438">
   <si>
     <t>楼层</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -887,10 +887,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>布置间距（mm）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1608,6 +1604,14 @@
   </si>
   <si>
     <t>无障碍卧室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房间外是否需要布置电子巡更</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1948,7 +1952,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2448,7 +2452,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2937,17 +2941,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29.25" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2961,7 +2965,7 @@
         <v>255</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2974,8 +2978,8 @@
       <c r="C2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="4">
-        <v>25000</v>
+      <c r="D2" s="4" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2988,8 +2992,8 @@
       <c r="C3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4">
-        <v>25000</v>
+      <c r="D3" s="4" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3002,8 +3006,8 @@
       <c r="C4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="4">
-        <v>25000</v>
+      <c r="D4" s="4" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3016,8 +3020,8 @@
       <c r="C5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="4">
-        <v>25000</v>
+      <c r="D5" s="4" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3030,13 +3034,154 @@
       <c r="C6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="4">
-        <v>25000</v>
+      <c r="D6" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3044,8 +3189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3173,9 +3318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E128" sqref="E128"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3188,56 +3333,56 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3247,7 +3392,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3255,188 +3400,188 @@
         <v>87</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D19" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D20" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D23" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D24" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D25" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D26" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D28" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D29" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D30" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D31" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D32" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D34" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D35" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D37" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D38" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -3454,115 +3599,115 @@
         <v>90</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D47" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D48" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D49" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D50" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D51" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D52" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D53" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D54" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D55" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D56" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D57" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D58" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D59" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
@@ -3570,7 +3715,7 @@
         <v>91</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.2">
@@ -3578,7 +3723,7 @@
         <v>92</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
@@ -3588,42 +3733,42 @@
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D63" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D64" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="D65" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D66" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>342</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D67" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
@@ -3631,31 +3776,31 @@
         <v>94</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D69" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D70" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="71" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="D71" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
@@ -3717,10 +3862,10 @@
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.2">
@@ -3728,12 +3873,12 @@
         <v>108</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D83" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.2">
@@ -3797,42 +3942,42 @@
         <v>121</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D95" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="96" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D96" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D98" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D99" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D100" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D101" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
@@ -3887,7 +4032,7 @@
     </row>
     <row r="112" spans="2:5" ht="57" x14ac:dyDescent="0.2">
       <c r="D112" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>132</v>
@@ -3908,10 +4053,10 @@
     </row>
     <row r="115" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -3919,12 +4064,12 @@
         <v>136</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3932,15 +4077,15 @@
         <v>137</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D119" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>371</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3948,25 +4093,25 @@
         <v>138</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B122" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -3979,7 +4124,7 @@
         <v>140</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -3987,7 +4132,7 @@
         <v>141</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -4010,7 +4155,7 @@
         <v>145</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="131" spans="2:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -4018,7 +4163,7 @@
         <v>146</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.2">
@@ -4033,10 +4178,10 @@
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B134" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E134" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.2">
@@ -4044,7 +4189,7 @@
         <v>149</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.2">
@@ -4078,7 +4223,7 @@
         <v>156</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.2">
@@ -4101,7 +4246,7 @@
         <v>160</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.2">
@@ -4114,7 +4259,7 @@
         <v>162</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.2">
@@ -4127,7 +4272,7 @@
         <v>164</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.2">
@@ -4137,12 +4282,12 @@
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D150" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D151" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.2">
@@ -4172,23 +4317,23 @@
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C157" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C158" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E158" s="3" t="s">
         <v>392</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C159" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E159" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.2">
@@ -4276,7 +4421,7 @@
         <v>187</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="177" spans="2:5" x14ac:dyDescent="0.2">
@@ -4324,7 +4469,7 @@
         <v>196</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="186" spans="2:5" x14ac:dyDescent="0.2">
@@ -4337,7 +4482,7 @@
         <v>198</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="188" spans="2:5" x14ac:dyDescent="0.2">
@@ -4345,36 +4490,36 @@
         <v>199</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="189" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C189" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="190" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D190" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E190" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="E190" s="3" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="191" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D191" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E191" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="E191" s="3" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="192" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D192" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E192" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="193" spans="2:5" x14ac:dyDescent="0.2">
@@ -4382,7 +4527,7 @@
         <v>200</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.2">
@@ -4390,7 +4535,7 @@
         <v>201</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="195" spans="2:5" x14ac:dyDescent="0.2">
@@ -4437,7 +4582,7 @@
     </row>
     <row r="201" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B201" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="202" spans="2:5" x14ac:dyDescent="0.2">
@@ -4445,7 +4590,7 @@
         <v>212</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="203" spans="2:5" x14ac:dyDescent="0.2">
@@ -4458,7 +4603,7 @@
         <v>214</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.2">
@@ -4466,7 +4611,7 @@
         <v>215</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="206" spans="2:5" x14ac:dyDescent="0.2">
@@ -4490,7 +4635,7 @@
         <v>220</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -4498,90 +4643,90 @@
         <v>221</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D210" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E210" s="3" t="s">
         <v>415</v>
-      </c>
-      <c r="E210" s="3" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D211" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E211" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="E211" s="3" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B213" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C214" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C215" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B216" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E216" s="3" t="s">
         <v>423</v>
-      </c>
-      <c r="E216" s="3" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C217" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C218" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E218" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="E218" s="3" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B219" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E219" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="E219" s="3" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C220" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C221" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C222" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E222" s="3" t="s">
         <v>432</v>
-      </c>
-      <c r="E222" s="3" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -4645,7 +4790,7 @@
     </row>
     <row r="234" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C234" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="235" spans="2:5" x14ac:dyDescent="0.2">
@@ -4681,7 +4826,7 @@
         <v>241</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.2">
@@ -4689,7 +4834,7 @@
         <v>242</v>
       </c>
       <c r="E241" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
commit layout Guard Tour System step3 (#497)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/上海地区住宅-安防配置表.xlsx
+++ b/AutoLoader/Contents/Support/上海地区住宅-安防配置表.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="438">
   <si>
     <t>楼层</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2941,10 +2941,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>375</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>162</v>
+        <v>381</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>399</v>
+        <v>184</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>200</v>
+        <v>399</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -3124,7 +3124,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>408</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>129</v>
+        <v>408</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
@@ -3175,6 +3175,20 @@
         <v>436</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>